<commit_message>
final fixes before submiting
</commit_message>
<xml_diff>
--- a/Project47/Results/Results.xlsx
+++ b/Project47/Results/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amita\source\repos\Project47\Project47\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23249208-9355-4981-AEDE-DA4D674C8F74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BDF208-A1F8-407E-ADDD-63DA8ABD577C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5316" yWindow="3456" windowWidth="22452" windowHeight="10188" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Habit1" sheetId="1" r:id="rId1"/>
@@ -22,12 +22,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>P</t>
   </si>
   <si>
     <t>Results</t>
+  </si>
+  <si>
+    <t>ApplicationCount</t>
   </si>
 </sst>
 </file>
@@ -978,7 +981,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Results</c:v>
+                  <c:v>ApplicationCount</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1002,16 +1005,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>7.4999999999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.08</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.5000000000000006E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.1</c:v>
@@ -1041,19 +1044,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.98599999999999999</c:v>
+                  <c:v>0.95599999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.66600000000000004</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.41399999999999998</c:v>
+                  <c:v>0.98799999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.2E-2</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
@@ -3791,8 +3794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{674CD9F3-0939-4174-A4EB-34F61E3A4C6C}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3802,16 +3805,16 @@
         <v>0</v>
       </c>
       <c r="B1">
+        <v>0.01</v>
+      </c>
+      <c r="C1">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D1">
+        <v>0.05</v>
+      </c>
+      <c r="E1">
         <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="C1">
-        <v>0.08</v>
-      </c>
-      <c r="D1">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="E1">
-        <v>0.09</v>
       </c>
       <c r="F1">
         <v>0.1</v>
@@ -3834,22 +3837,22 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>0.98599999999999999</v>
-      </c>
-      <c r="C2">
-        <v>0.9</v>
-      </c>
       <c r="D2">
-        <v>0.66600000000000004</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>0.41399999999999998</v>
+        <v>0.98799999999999999</v>
       </c>
       <c r="F2">
-        <v>6.2E-2</v>
+        <v>0.08</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -3877,7 +3880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23F5F97F-B42B-4756-936B-932209898FC3}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:K2"/>
     </sheetView>
   </sheetViews>

</xml_diff>